<commit_message>
:cat: Early development stage - chaos
開発初期段階につき仕様ふわっふわで新陳代謝が早いので特に意味の無い保険コミット
</commit_message>
<xml_diff>
--- a/Data/BoneCoordinates.xlsx
+++ b/Data/BoneCoordinates.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
   <si>
     <t>センター</t>
   </si>
@@ -179,6 +180,118 @@
   </si>
   <si>
     <t>Matching target</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Z</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Parent</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>上半身</t>
+    <rPh sb="0" eb="3">
+      <t>ジョウハンシン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>首</t>
+    <rPh sb="0" eb="1">
+      <t>クビ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>右腕</t>
+    <rPh sb="0" eb="2">
+      <t>ミギウデ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>右ひじ</t>
+    <rPh sb="0" eb="1">
+      <t>ミギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>左腕</t>
+    <rPh sb="0" eb="2">
+      <t>ヒダリウデ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>左ひじ</t>
+    <rPh sb="0" eb="1">
+      <t>ヒダリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>センター</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>右足</t>
+    <rPh sb="0" eb="2">
+      <t>ミギアシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>右ひざ</t>
+    <rPh sb="0" eb="1">
+      <t>ミギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>右足首</t>
+    <rPh sb="0" eb="3">
+      <t>ミギアシクビ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>左足</t>
+    <rPh sb="0" eb="2">
+      <t>ヒダリアシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>左ひざ</t>
+    <rPh sb="0" eb="1">
+      <t>ヒダリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>左足首</t>
+    <rPh sb="0" eb="3">
+      <t>ヒダリアシクビ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>From parent to child</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -186,6 +299,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -400,7 +516,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -459,6 +575,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -755,19 +877,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="5.375" customWidth="1"/>
-    <col min="8" max="8" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="7" customWidth="1"/>
+    <col min="12" max="12" width="14.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -775,21 +898,27 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:12">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="18" t="s">
+      <c r="K2" s="16"/>
+      <c r="L2" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:12">
       <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
@@ -803,525 +932,819 @@
       <c r="E3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="K3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="L3" s="19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:12">
       <c r="A4" s="9">
         <v>1</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="20">
         <v>0</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="20">
         <v>7.8325899999999997</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="20">
         <v>0</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="K4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="L4" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="9">
         <v>2</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="20">
         <v>0</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="20">
         <v>16.904699999999998</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="20">
         <v>9.5379980000000003E-2</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="10" t="s">
+      <c r="F5" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="20">
+        <f ca="1">C5-OFFSET(C$4,MATCH($F5,$B$4:$B$22,0)-1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="20">
+        <f t="shared" ref="H5:I5" ca="1" si="0">D5-OFFSET(D$4,MATCH($F5,$B$4:$B$22,0)-1,0)</f>
+        <v>3.6043699999999976</v>
+      </c>
+      <c r="I5" s="20">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.40433527999999996</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="L5" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="9">
         <v>3</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="20">
         <v>-0.41408929999999999</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="20">
         <v>17.99653</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="20">
         <v>-0.50448780000000004</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="12">
+      <c r="F6" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="20">
+        <f t="shared" ref="G6:G22" ca="1" si="1">C6-OFFSET(C$4,MATCH($F6,$B$4:$B$22,0)-1,0)</f>
+        <v>-0.41408929999999999</v>
+      </c>
+      <c r="H6" s="20">
+        <f t="shared" ref="H6:H22" ca="1" si="2">D6-OFFSET(D$4,MATCH($F6,$B$4:$B$22,0)-1,0)</f>
+        <v>1.0918300000000016</v>
+      </c>
+      <c r="I6" s="20">
+        <f t="shared" ref="I6:I22" ca="1" si="3">E6-OFFSET(E$4,MATCH($F6,$B$4:$B$22,0)-1,0)</f>
+        <v>-0.59986778000000007</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="12">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:12">
       <c r="A7" s="9">
         <v>4</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="20">
         <v>0.41408929999999999</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="20">
         <v>17.99653</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="20">
         <v>-0.50448780000000004</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="12">
+      <c r="F7" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.41408929999999999</v>
+      </c>
+      <c r="H7" s="20">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.0918300000000016</v>
+      </c>
+      <c r="I7" s="20">
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.59986778000000007</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="12">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:12">
       <c r="A8" s="9">
         <v>5</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="20">
         <v>-1.34683</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="20">
         <v>16.195910000000001</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="20">
         <v>-4.8119990000000001E-2</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="F8" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="20">
+        <f t="shared" ca="1" si="1"/>
+        <v>-1.34683</v>
+      </c>
+      <c r="H8" s="20">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.70878999999999692</v>
+      </c>
+      <c r="I8" s="20">
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.14349997</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="12">
+      <c r="L8" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:12">
       <c r="A9" s="9">
         <v>6</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="20">
         <v>-3.53281</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="20">
         <v>14.483890000000001</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="20">
         <v>-4.8119990000000001E-2</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="10" t="s">
+      <c r="F9" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="20">
+        <f t="shared" ca="1" si="1"/>
+        <v>-2.1859799999999998</v>
+      </c>
+      <c r="H9" s="20">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.7120200000000008</v>
+      </c>
+      <c r="I9" s="20">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="12">
+      <c r="L9" s="12">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:12">
       <c r="A10" s="9">
         <v>7</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="20">
         <v>-5.2831200000000003</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="20">
         <v>13.126760000000001</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="20">
         <v>8.801001E-2</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="12">
+      <c r="F10" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="20">
+        <f t="shared" ca="1" si="1"/>
+        <v>-1.7503100000000003</v>
+      </c>
+      <c r="H10" s="20">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.3571299999999997</v>
+      </c>
+      <c r="I10" s="20">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.13613</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="12">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:12">
       <c r="A11" s="9">
         <v>8</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="20">
         <v>1.34683</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="20">
         <v>16.195910000000001</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="20">
         <v>-4.8119990000000001E-2</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="10" t="s">
+      <c r="F11" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="20">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.34683</v>
+      </c>
+      <c r="H11" s="20">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.70878999999999692</v>
+      </c>
+      <c r="I11" s="20">
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.14349997</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="12">
+      <c r="L11" s="12">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:12">
       <c r="A12" s="9">
         <v>9</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="20">
         <v>3.53281</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="20">
         <v>14.483890000000001</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="20">
         <v>-4.8119990000000001E-2</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="10" t="s">
+      <c r="F12" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="20">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.1859799999999998</v>
+      </c>
+      <c r="H12" s="20">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.7120200000000008</v>
+      </c>
+      <c r="I12" s="20">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="12">
+      <c r="L12" s="12">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:12">
       <c r="A13" s="9">
         <v>10</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="20">
         <v>5.2831200000000003</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="20">
         <v>13.126760000000001</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="20">
         <v>8.801001E-2</v>
       </c>
-      <c r="F13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="12">
+      <c r="F13" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="20">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.7503100000000003</v>
+      </c>
+      <c r="H13" s="20">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.3571299999999997</v>
+      </c>
+      <c r="I13" s="20">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.13613</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" s="12">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:12">
       <c r="A14" s="9">
         <v>11</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="20">
         <v>-1.01084</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="20">
         <v>11.194660000000001</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="20">
         <v>-0.37495000000000001</v>
       </c>
-      <c r="F14" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="10" t="s">
+      <c r="F14" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="20">
+        <f t="shared" ca="1" si="1"/>
+        <v>-1.01084</v>
+      </c>
+      <c r="H14" s="20">
+        <f t="shared" ca="1" si="2"/>
+        <v>3.362070000000001</v>
+      </c>
+      <c r="I14" s="20">
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.37495000000000001</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="12">
+      <c r="L14" s="12">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:12">
       <c r="A15" s="9">
         <v>12</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="20">
         <v>-0.71670999999999996</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="20">
         <v>6.5126299999999997</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="20">
         <v>-0.35964000000000002</v>
       </c>
-      <c r="F15" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="10" t="s">
+      <c r="F15" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.29413</v>
+      </c>
+      <c r="H15" s="20">
+        <f t="shared" ca="1" si="2"/>
+        <v>-4.682030000000001</v>
+      </c>
+      <c r="I15" s="20">
+        <f t="shared" ca="1" si="3"/>
+        <v>1.530999999999999E-2</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="12">
+      <c r="L15" s="12">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:12">
       <c r="A16" s="9">
         <v>13</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="20">
         <v>-0.77115489999999998</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="20">
         <v>1.5822099999999999</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="20">
         <v>2.6919990000000001E-2</v>
       </c>
-      <c r="F16" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="10" t="s">
+      <c r="F16" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="20">
+        <f t="shared" ca="1" si="1"/>
+        <v>-5.4444900000000018E-2</v>
+      </c>
+      <c r="H16" s="20">
+        <f t="shared" ca="1" si="2"/>
+        <v>-4.9304199999999998</v>
+      </c>
+      <c r="I16" s="20">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.38655999000000002</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="12">
+      <c r="L16" s="12">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:12">
       <c r="A17" s="9">
         <v>14</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="20">
         <v>-0.81474000000000002</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="20">
         <v>0.3968101</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="20">
         <v>-2.1573899999999999</v>
       </c>
-      <c r="F17" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H17" s="12">
+      <c r="F17" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="20">
+        <f t="shared" ca="1" si="1"/>
+        <v>-4.3585100000000043E-2</v>
+      </c>
+      <c r="H17" s="20">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.1853999</v>
+      </c>
+      <c r="I17" s="20">
+        <f t="shared" ca="1" si="3"/>
+        <v>-2.18430999</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" s="12">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:12">
       <c r="A18" s="9">
         <v>15</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="20">
         <v>1.01084</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="20">
         <v>11.194660000000001</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="20">
         <v>-0.37495000000000001</v>
       </c>
-      <c r="F18" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="10" t="s">
+      <c r="F18" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" s="20">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.01084</v>
+      </c>
+      <c r="H18" s="20">
+        <f t="shared" ca="1" si="2"/>
+        <v>3.362070000000001</v>
+      </c>
+      <c r="I18" s="20">
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.37495000000000001</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="12">
+      <c r="L18" s="12">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:12">
       <c r="A19" s="9">
         <v>16</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="20">
         <v>0.71670999999999996</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="20">
         <v>6.5126299999999997</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="20">
         <v>-0.35964000000000002</v>
       </c>
-      <c r="F19" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19" s="10" t="s">
+      <c r="F19" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="20">
+        <f t="shared" ca="1" si="1"/>
+        <v>-0.29413</v>
+      </c>
+      <c r="H19" s="20">
+        <f t="shared" ca="1" si="2"/>
+        <v>-4.682030000000001</v>
+      </c>
+      <c r="I19" s="20">
+        <f t="shared" ca="1" si="3"/>
+        <v>1.530999999999999E-2</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="12">
+      <c r="L19" s="12">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:12">
       <c r="A20" s="9">
         <v>17</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="20">
         <v>0.77115489999999998</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="20">
         <v>1.5822099999999999</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="20">
         <v>2.6919990000000001E-2</v>
       </c>
-      <c r="F20" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" s="10" t="s">
+      <c r="F20" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" s="20">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.4444900000000018E-2</v>
+      </c>
+      <c r="H20" s="20">
+        <f t="shared" ca="1" si="2"/>
+        <v>-4.9304199999999998</v>
+      </c>
+      <c r="I20" s="20">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.38655999000000002</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H20" s="12">
+      <c r="L20" s="12">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:12">
       <c r="A21" s="9">
         <v>18</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="20">
         <v>0.81474000000000002</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="20">
         <v>0.3968101</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="20">
         <v>-2.1573899999999999</v>
       </c>
-      <c r="F21" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H21" s="12">
+      <c r="F21" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" s="20">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.3585100000000043E-2</v>
+      </c>
+      <c r="H21" s="20">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.1853999</v>
+      </c>
+      <c r="I21" s="20">
+        <f t="shared" ca="1" si="3"/>
+        <v>-2.18430999</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L21" s="12">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:12">
       <c r="A22" s="13">
         <v>19</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="21">
         <v>0</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="21">
         <v>13.300330000000001</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="21">
         <v>-0.30895529999999999</v>
       </c>
-      <c r="F22" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="G22" s="14" t="s">
+      <c r="F22" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="21">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.4677400000000009</v>
+      </c>
+      <c r="I22" s="21">
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.30895529999999999</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="F23" s="4" t="s">
+      <c r="L22" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="J23" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G23" s="1">
-        <f>COUNTIF(F4:G22,"=y")</f>
+      <c r="K23" s="1">
+        <f>COUNTIF(J4:K22,"=y")</f>
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
-      <c r="F24" s="3" t="s">
+    <row r="24" spans="1:12">
+      <c r="J24" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G24" s="2">
-        <f>G23*3</f>
+      <c r="K24" s="2">
+        <f>K23*3</f>
         <v>42</v>
       </c>
     </row>

</xml_diff>